<commit_message>
Burndown chart and sprint backlog updated. Code smells Martim Costa
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 1/Sprint1/Burndown chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Ambiente de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\IdeaProjects\ganttproject\Project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01433005-4E25-4A87-A6F2-86E0A1B5783A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E528E31B-AA4D-4965-9DB3-FA4C1D34896F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,7 +716,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -829,13 +829,13 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2090,7 +2090,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2186,7 +2186,9 @@
       <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
@@ -2218,7 +2220,9 @@
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9">
+        <v>0.4</v>
+      </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
@@ -2272,7 +2276,7 @@
       </c>
       <c r="G11" s="13">
         <f>SUM(G6:G10)</f>
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="H11" s="13">
         <f>SUM(H6:H10)</f>
@@ -2303,15 +2307,15 @@
       </c>
       <c r="G12" s="14">
         <f>F12-SUM(G6:G10)</f>
-        <v>7</v>
+        <v>5.6</v>
       </c>
       <c r="H12" s="14">
         <f>G12-SUM(H6:H10)</f>
-        <v>7</v>
+        <v>5.6</v>
       </c>
       <c r="I12" s="14">
         <f>H12-SUM(I6:I10)</f>
-        <v>7</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Patterns -Martim Costa. Burndown chart and sprint chart updated
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 1/Sprint1/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\IdeaProjects\ganttproject\Project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E528E31B-AA4D-4965-9DB3-FA4C1D34896F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E03CF6-7629-42F2-91D7-11E029C46F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,7 +719,7 @@
                   <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -832,10 +832,10 @@
                   <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6</c:v>
+                  <c:v>5.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6</c:v>
+                  <c:v>5.1999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2090,7 +2090,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2205,7 +2205,9 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9">
+        <v>0.4</v>
+      </c>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
@@ -2280,7 +2282,7 @@
       </c>
       <c r="H11" s="13">
         <f>SUM(H6:H10)</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I11" s="13">
         <f>SUM(I6:I10)</f>
@@ -2311,11 +2313,11 @@
       </c>
       <c r="H12" s="14">
         <f>G12-SUM(H6:H10)</f>
-        <v>5.6</v>
+        <v>5.1999999999999993</v>
       </c>
       <c r="I12" s="14">
         <f>H12-SUM(I6:I10)</f>
-        <v>5.6</v>
+        <v>5.1999999999999993</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Burndown chart and sprint log update
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 1/Sprint1/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\IdeaProjects\ganttproject\Project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E03CF6-7629-42F2-91D7-11E029C46F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6860AD-45A3-4114-9C4E-20A3F860DB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -719,7 +719,7 @@
                   <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -832,10 +832,10 @@
                   <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1999999999999993</c:v>
+                  <c:v>3.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1999999999999993</c:v>
+                  <c:v>3.5999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2089,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2206,7 +2206,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -2225,7 +2225,9 @@
       <c r="G8" s="9">
         <v>0.4</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9">
+        <v>0.8</v>
+      </c>
       <c r="I8" s="9"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -2282,7 +2284,7 @@
       </c>
       <c r="H11" s="13">
         <f>SUM(H6:H10)</f>
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="13">
         <f>SUM(I6:I10)</f>
@@ -2313,11 +2315,11 @@
       </c>
       <c r="H12" s="14">
         <f>G12-SUM(H6:H10)</f>
-        <v>5.1999999999999993</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="I12" s="14">
         <f>H12-SUM(I6:I10)</f>
-        <v>5.1999999999999993</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Burndown chart and sprint log grammar fixes
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 1/Sprint1/Burndown chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\IdeaProjects\ganttproject\Project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232AC5C0-0247-4363-8173-8E38EAFEE5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D402185D-25E3-4E95-860B-4E17BCC1BEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Task ID</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Preparation of the "workplace"</t>
   </si>
   <si>
-    <t>Identifie GoF design patterns</t>
-  </si>
-  <si>
     <t>Identifie code smells</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>Make report</t>
+  </si>
+  <si>
+    <t>Identify GoF design patterns</t>
+  </si>
+  <si>
+    <t>Identify code smells</t>
   </si>
 </sst>
 </file>
@@ -2089,8 +2092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2197,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7" s="25">
         <v>2</v>
@@ -2217,7 +2220,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="25">
         <v>2</v>
@@ -2239,7 +2242,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="25">
         <v>1</v>
@@ -2257,7 +2260,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="26">
         <v>1</v>

</xml_diff>